<commit_message>
Minor changes to documentation
</commit_message>
<xml_diff>
--- a/documents/SOEN 6011 Skill Selection Sheet.xlsx
+++ b/documents/SOEN 6011 Skill Selection Sheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\soen6011\project\SESTOPIA\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhruv\Documents\GitHub\SESTOPIA\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416AC204-AE33-4459-8509-A149998A52A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,16 +108,16 @@
     <t>Computing Foundations</t>
   </si>
   <si>
-    <t>Algorithms and Complexity</t>
-  </si>
-  <si>
     <t>Data Analysis</t>
+  </si>
+  <si>
+    <t>Algorithms and Complexity Analysis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -401,21 +402,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="50.109375" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
@@ -481,7 +482,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1">
@@ -514,7 +515,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
resolution for home page done- skills added
</commit_message>
<xml_diff>
--- a/documents/SOEN 6011 Skill Selection Sheet.xlsx
+++ b/documents/SOEN 6011 Skill Selection Sheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\soen6011\project\SESTOPIA\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhruv\Documents\GitHub\SESTOPIA\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416AC204-AE33-4459-8509-A149998A52A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,16 +108,16 @@
     <t>Computing Foundations</t>
   </si>
   <si>
-    <t>Algorithms and Complexity</t>
-  </si>
-  <si>
     <t>Data Analysis</t>
+  </si>
+  <si>
+    <t>Algorithms and Complexity Analysis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="10"/>
@@ -401,21 +402,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
-    <col min="2" max="2" width="50.109375" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
@@ -481,7 +482,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1">
@@ -514,7 +515,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
database dump file and document update
</commit_message>
<xml_diff>
--- a/documents/SOEN 6011 Skill Selection Sheet.xlsx
+++ b/documents/SOEN 6011 Skill Selection Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhruv\Documents\GitHub\SESTOPIA\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0.Work\Graduate\front\SESTOPIA\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416AC204-AE33-4459-8509-A149998A52A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92198ADC-6F09-40AD-9F95-C7484F8435E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1824" yWindow="2904" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,34 +91,24 @@
     <t>Dhruv Goyani</t>
   </si>
   <si>
-    <r>
-      <t>API</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> design and programming</t>
-    </r>
+    <t>Computing Foundations</t>
+  </si>
+  <si>
+    <t>Data Analysis</t>
+  </si>
+  <si>
+    <t>Algorithms and Complexity Analysis</t>
+  </si>
+  <si>
+    <t>Restful API programming</t>
     <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Computing Foundations</t>
-  </si>
-  <si>
-    <t>Data Analysis</t>
-  </si>
-  <si>
-    <t>Algorithms and Complexity Analysis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -190,7 +180,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -412,14 +402,14 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="50.109375" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -441,7 +431,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -452,7 +442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -463,7 +453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -474,7 +464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -482,10 +472,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -493,10 +483,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -507,128 +497,128 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>

</xml_diff>